<commit_message>
fix broken mapping_orig.txt links
https://knights-lab.github.io/MLRepo/docs/datasets/claesson/mapping-orig
.txt
to
https://github.com/knights-lab/MLRepo/blob/master/datasets/claesson/mapp
ing-orig.txt
</commit_message>
<xml_diff>
--- a/web/data/dataset_metadata.xlsx
+++ b/web/data/dataset_metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="39620" windowHeight="22080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_metadata" sheetId="1" r:id="rId1"/>
@@ -1721,9 +1721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1854,8 +1854,8 @@
         <v>10</v>
       </c>
       <c r="R2" s="10" t="str">
-        <f>CONCATENATE("./datasets/", B2, "/mapping-orig.txt")</f>
-        <v>./datasets/cho/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B2, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/cho/mapping-orig.txt</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -1908,8 +1908,8 @@
         <v>10</v>
       </c>
       <c r="R3" s="10" t="str">
-        <f t="shared" ref="R3:R16" si="0">CONCATENATE("./datasets/", B3, "/mapping-orig.txt")</f>
-        <v>./datasets/claesson/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B3, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/claesson/mapping-orig.txt</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -1965,8 +1965,8 @@
         <v>24</v>
       </c>
       <c r="R4" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/david/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B4, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/david/mapping-orig.txt</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -2019,8 +2019,8 @@
         <v>10</v>
       </c>
       <c r="R5" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/gevers/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B5, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/gevers/mapping-orig.txt</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -2076,8 +2076,8 @@
         <v>10</v>
       </c>
       <c r="R6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/hmp/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B6, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/hmp/mapping-orig.txt</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -2133,8 +2133,8 @@
         <v>41</v>
       </c>
       <c r="R7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/kostic/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B7, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/kostic/mapping-orig.txt</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2187,8 +2187,8 @@
         <v>10</v>
       </c>
       <c r="R8" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/bacteremia/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B8, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/bacteremia/mapping-orig.txt</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2244,8 +2244,8 @@
         <v>10</v>
       </c>
       <c r="R9" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/sokol/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B9, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/sokol/mapping-orig.txt</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -2298,8 +2298,8 @@
         <v>10</v>
       </c>
       <c r="R10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/turnbaugh_twins/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B10, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/turnbaugh_twins/mapping-orig.txt</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2355,8 +2355,8 @@
         <v>24</v>
       </c>
       <c r="R11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/bushman_cafe/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B11, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/bushman_cafe/mapping-orig.txt</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2412,8 +2412,8 @@
         <v>10</v>
       </c>
       <c r="R12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/yatsunenko/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B12, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/yatsunenko/mapping-orig.txt</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2466,8 +2466,8 @@
         <v>10</v>
       </c>
       <c r="R13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/ravel/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B13, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/ravel/mapping-orig.txt</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2520,8 +2520,8 @@
         <v>10</v>
       </c>
       <c r="R14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/karlsson/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B14, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/karlsson/mapping-orig.txt</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2574,8 +2574,8 @@
         <v>10</v>
       </c>
       <c r="R15" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/qin2012/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B15, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/qin2012/mapping-orig.txt</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2628,8 +2628,8 @@
         <v>10</v>
       </c>
       <c r="R16" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>./datasets/qin2014/mapping-orig.txt</v>
+        <f>CONCATENATE("../../blob/master/datasets/", B16, "/mapping-orig.txt")</f>
+        <v>../../blob/master/datasets/qin2014/mapping-orig.txt</v>
       </c>
     </row>
   </sheetData>
@@ -2642,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O34" sqref="O34"/>
     </sheetView>

</xml_diff>

<commit_message>
Revert "fix broken mapping_orig.txt links"
This reverts commit 5378006d9595cfc87e9b5edafb1224d4c824809c.
</commit_message>
<xml_diff>
--- a/web/data/dataset_metadata.xlsx
+++ b/web/data/dataset_metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="39620" windowHeight="22080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_metadata" sheetId="1" r:id="rId1"/>
@@ -1721,9 +1721,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R17" sqref="R17"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1854,8 +1854,8 @@
         <v>10</v>
       </c>
       <c r="R2" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B2, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/cho/mapping-orig.txt</v>
+        <f>CONCATENATE("./datasets/", B2, "/mapping-orig.txt")</f>
+        <v>./datasets/cho/mapping-orig.txt</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
@@ -1908,8 +1908,8 @@
         <v>10</v>
       </c>
       <c r="R3" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B3, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/claesson/mapping-orig.txt</v>
+        <f t="shared" ref="R3:R16" si="0">CONCATENATE("./datasets/", B3, "/mapping-orig.txt")</f>
+        <v>./datasets/claesson/mapping-orig.txt</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -1965,8 +1965,8 @@
         <v>24</v>
       </c>
       <c r="R4" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B4, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/david/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/david/mapping-orig.txt</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -2019,8 +2019,8 @@
         <v>10</v>
       </c>
       <c r="R5" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B5, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/gevers/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/gevers/mapping-orig.txt</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -2076,8 +2076,8 @@
         <v>10</v>
       </c>
       <c r="R6" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B6, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/hmp/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/hmp/mapping-orig.txt</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
@@ -2133,8 +2133,8 @@
         <v>41</v>
       </c>
       <c r="R7" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B7, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/kostic/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/kostic/mapping-orig.txt</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2187,8 +2187,8 @@
         <v>10</v>
       </c>
       <c r="R8" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B8, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/bacteremia/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/bacteremia/mapping-orig.txt</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2244,8 +2244,8 @@
         <v>10</v>
       </c>
       <c r="R9" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B9, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/sokol/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/sokol/mapping-orig.txt</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -2298,8 +2298,8 @@
         <v>10</v>
       </c>
       <c r="R10" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B10, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/turnbaugh_twins/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/turnbaugh_twins/mapping-orig.txt</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2355,8 +2355,8 @@
         <v>24</v>
       </c>
       <c r="R11" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B11, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/bushman_cafe/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/bushman_cafe/mapping-orig.txt</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2412,8 +2412,8 @@
         <v>10</v>
       </c>
       <c r="R12" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B12, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/yatsunenko/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/yatsunenko/mapping-orig.txt</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2466,8 +2466,8 @@
         <v>10</v>
       </c>
       <c r="R13" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B13, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/ravel/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/ravel/mapping-orig.txt</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2520,8 +2520,8 @@
         <v>10</v>
       </c>
       <c r="R14" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B14, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/karlsson/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/karlsson/mapping-orig.txt</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2574,8 +2574,8 @@
         <v>10</v>
       </c>
       <c r="R15" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B15, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/qin2012/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/qin2012/mapping-orig.txt</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="18" x14ac:dyDescent="0.25">
@@ -2628,8 +2628,8 @@
         <v>10</v>
       </c>
       <c r="R16" s="10" t="str">
-        <f>CONCATENATE("../../blob/master/datasets/", B16, "/mapping-orig.txt")</f>
-        <v>../../blob/master/datasets/qin2014/mapping-orig.txt</v>
+        <f t="shared" si="0"/>
+        <v>./datasets/qin2014/mapping-orig.txt</v>
       </c>
     </row>
   </sheetData>
@@ -2642,7 +2642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O34" sqref="O34"/>
     </sheetView>

</xml_diff>